<commit_message>
The Project has been finished but some dependency needs to be removed and programme must be efficient
</commit_message>
<xml_diff>
--- a/Parent_Notification/Sample Data/Parent Data.xlsx
+++ b/Parent_Notification/Sample Data/Parent Data.xlsx
@@ -393,7 +393,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +543,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>8368648022</v>
+        <v>9582566693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>